<commit_message>
Add a test (although overall suite doesn't pass yet)
</commit_message>
<xml_diff>
--- a/tests/framework_init_zero.xlsx
+++ b/tests/framework_init_zero.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romesh.abeysuriya/projects/atomica/atomica/library/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh\projects\atomica\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FAF1E9-4E8C-A64F-8459-8B25E7C418FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AEE670-C93E-412B-95D6-17FC29AC8AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="28560" windowHeight="14180" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14940" yWindow="1455" windowWidth="31635" windowHeight="16380" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -553,7 +553,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -1040,7 +1040,7 @@
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -1415,13 +1415,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="97.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="97.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="234.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1437,22 +1437,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1513,13 +1513,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1543,35 +1543,35 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
     </row>
@@ -1586,19 +1586,19 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="166" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>40</v>
       </c>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>46</v>
       </c>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>48</v>
       </c>
@@ -1748,7 +1748,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1793,9 +1793,9 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>dead_other</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f>Compartments!$A$2</f>
         <v>source</v>
@@ -1858,7 +1858,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>Compartments!$A$3</f>
         <v>sus</v>
@@ -1880,7 +1880,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>Compartments!$A$4</f>
         <v>vac</v>
@@ -1898,7 +1898,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>Compartments!$A$5</f>
         <v>undx</v>
@@ -1922,7 +1922,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f>Compartments!$A$6</f>
         <v>dx</v>
@@ -1946,7 +1946,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>Compartments!$A$7</f>
         <v>tx</v>
@@ -1972,7 +1972,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f>Compartments!$A$8</f>
         <v>lost</v>
@@ -1996,7 +1996,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>Compartments!$A$9</f>
         <v>txs</v>
@@ -2022,7 +2022,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f>Compartments!$A$10</f>
         <v>dead_tb</v>
@@ -2038,7 +2038,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f>Compartments!$A$11</f>
         <v>dead_other</v>
@@ -2070,19 +2070,19 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="165" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2098,8 +2098,11 @@
       <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>68</v>
       </c>
@@ -2115,12 +2118,14 @@
       <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3">
+        <v>1000</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>71</v>
       </c>
@@ -2136,8 +2141,11 @@
       <c r="E3" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>74</v>
       </c>
@@ -2147,14 +2155,10 @@
       <c r="C4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
@@ -2170,8 +2174,11 @@
       <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>80</v>
       </c>
@@ -2181,14 +2188,10 @@
       <c r="C6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>83</v>
       </c>
@@ -2198,33 +2201,29 @@
       <c r="C7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
     </row>
   </sheetData>
@@ -2243,23 +2242,23 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F20"/>
+      <selection activeCell="G20" sqref="G20:G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2288,7 +2287,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -2298,6 +2297,9 @@
       <c r="C2" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="D2" s="3">
+        <v>1000</v>
+      </c>
       <c r="E2" s="3">
         <v>0</v>
       </c>
@@ -2308,7 +2310,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>93</v>
       </c>
@@ -2318,7 +2320,9 @@
       <c r="C3" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>100</v>
+      </c>
       <c r="E3" s="3">
         <v>0</v>
       </c>
@@ -2329,7 +2333,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>55</v>
       </c>
@@ -2352,7 +2356,7 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>57</v>
       </c>
@@ -2377,7 +2381,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>98</v>
       </c>
@@ -2387,7 +2391,9 @@
       <c r="C6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <v>50</v>
+      </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
@@ -2398,7 +2404,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>54</v>
       </c>
@@ -2421,7 +2427,7 @@
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>102</v>
       </c>
@@ -2431,7 +2437,9 @@
       <c r="C8" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3">
+        <v>50</v>
+      </c>
       <c r="E8" s="3">
         <v>0</v>
       </c>
@@ -2444,7 +2452,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>104</v>
       </c>
@@ -2467,7 +2475,7 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>107</v>
       </c>
@@ -2490,7 +2498,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>58</v>
       </c>
@@ -2513,7 +2521,7 @@
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>112</v>
       </c>
@@ -2523,7 +2531,9 @@
       <c r="C12" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7">
+        <v>50</v>
+      </c>
       <c r="E12" s="3">
         <v>0</v>
       </c>
@@ -2536,7 +2546,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>60</v>
       </c>
@@ -2559,7 +2569,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>61</v>
       </c>
@@ -2569,7 +2579,9 @@
       <c r="C14" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3">
+        <v>0.1</v>
+      </c>
       <c r="E14" s="3">
         <v>0</v>
       </c>
@@ -2582,7 +2594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>62</v>
       </c>
@@ -2607,7 +2619,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>64</v>
       </c>
@@ -2632,7 +2644,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
@@ -2656,7 +2668,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>63</v>
       </c>
@@ -2681,7 +2693,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>65</v>
       </c>
@@ -2706,7 +2718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>56</v>
       </c>
@@ -2730,7 +2742,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2740,7 +2752,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2750,7 +2762,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2760,7 +2772,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2770,7 +2782,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2780,17 +2792,17 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -2854,13 +2866,13 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>124</v>
       </c>
@@ -2868,7 +2880,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>72</v>
       </c>
@@ -2876,7 +2888,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>75</v>
       </c>
@@ -2884,7 +2896,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>78</v>
       </c>
@@ -2892,7 +2904,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>81</v>
       </c>
@@ -2903,7 +2915,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>84</v>
       </c>
@@ -2914,17 +2926,17 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>

</xml_diff>